<commit_message>
Edited the data with the correct column names
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data for Hospital Database.xlsx
+++ b/Documentation/Sample Data for Hospital Database.xlsx
@@ -1,22 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Spencer/Documents/CMSC508/Project/vcu-cs-cmsc508-teamproject-summer2020-team-10/Documentation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548C0C5-5082-2E41-A137-B491426140C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="15100" yWindow="0" windowWidth="13700" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Patients" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Departments" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Hospitals" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Doctors" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Hospital Personnel" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Emergency Contacts" sheetId="6" r:id="rId9"/>
+    <sheet name="Patients" sheetId="1" r:id="rId1"/>
+    <sheet name="Departments" sheetId="2" r:id="rId2"/>
+    <sheet name="Hospitals" sheetId="3" r:id="rId3"/>
+    <sheet name="Doctors" sheetId="4" r:id="rId4"/>
+    <sheet name="Hospital Personnel" sheetId="5" r:id="rId5"/>
+    <sheet name="Emergency Contacts" sheetId="6" r:id="rId6"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="354">
   <si>
     <t>hospital name</t>
   </si>
@@ -1075,33 +1084,37 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>doctor_ID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="mmm d, yyyy"/>
-    <numFmt numFmtId="165" formatCode="mmmm d, yyyy"/>
+    <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -1111,77 +1124,56 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1371,23 +1363,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="5" max="5" width="30.86"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1427,8 +1424,11 @@
       <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="N1" s="6" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -1445,10 +1445,10 @@
         <v>19</v>
       </c>
       <c r="F2" s="3">
-        <v>43703.0</v>
+        <v>43703</v>
       </c>
       <c r="G2" s="3">
-        <v>44161.0</v>
+        <v>44161</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
@@ -1457,7 +1457,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="4">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>23</v>
@@ -1466,10 +1466,13 @@
         <v>24</v>
       </c>
       <c r="M2" s="4">
-        <v>303.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>303</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
@@ -1486,10 +1489,10 @@
         <v>19</v>
       </c>
       <c r="F3" s="3">
-        <v>44119.0</v>
+        <v>44119</v>
       </c>
       <c r="G3" s="3">
-        <v>43911.0</v>
+        <v>43911</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>31</v>
@@ -1498,7 +1501,7 @@
         <v>32</v>
       </c>
       <c r="J3" s="4">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>23</v>
@@ -1507,10 +1510,13 @@
         <v>34</v>
       </c>
       <c r="M3" s="4">
-        <v>241.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>241</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1527,10 +1533,10 @@
         <v>19</v>
       </c>
       <c r="F4" s="3">
-        <v>44286.0</v>
+        <v>44286</v>
       </c>
       <c r="G4" s="3">
-        <v>44121.0</v>
+        <v>44121</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>21</v>
@@ -1539,7 +1545,7 @@
         <v>41</v>
       </c>
       <c r="J4" s="4">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>42</v>
@@ -1548,10 +1554,13 @@
         <v>43</v>
       </c>
       <c r="M4" s="4">
-        <v>128.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>128</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
@@ -1568,10 +1577,10 @@
         <v>49</v>
       </c>
       <c r="F5" s="3">
-        <v>43628.0</v>
+        <v>43628</v>
       </c>
       <c r="G5" s="3">
-        <v>44198.0</v>
+        <v>44198</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>50</v>
@@ -1580,7 +1589,7 @@
         <v>51</v>
       </c>
       <c r="J5" s="4">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>42</v>
@@ -1589,10 +1598,13 @@
         <v>52</v>
       </c>
       <c r="M5" s="4">
-        <v>368.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>368</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1609,10 +1621,10 @@
         <v>58</v>
       </c>
       <c r="F6" s="3">
-        <v>44266.0</v>
+        <v>44266</v>
       </c>
       <c r="G6" s="3">
-        <v>44279.0</v>
+        <v>44279</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>50</v>
@@ -1621,7 +1633,7 @@
         <v>61</v>
       </c>
       <c r="J6" s="4">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>23</v>
@@ -1630,27 +1642,31 @@
         <v>62</v>
       </c>
       <c r="M6" s="4">
-        <v>291.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>291</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="9" t="s">
         <v>67</v>
       </c>
+      <c r="D7" s="10"/>
       <c r="E7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="3">
-        <v>43826.0</v>
+        <v>43826</v>
       </c>
       <c r="G7" s="3">
-        <v>44138.0</v>
+        <v>44138</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>70</v>
@@ -1659,7 +1675,7 @@
         <v>61</v>
       </c>
       <c r="J7" s="4">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>42</v>
@@ -1668,10 +1684,13 @@
         <v>62</v>
       </c>
       <c r="M7" s="4">
-        <v>270.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>270</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
@@ -1688,10 +1707,10 @@
         <v>24</v>
       </c>
       <c r="F8" s="3">
-        <v>44166.0</v>
+        <v>44166</v>
       </c>
       <c r="G8" s="3">
-        <v>43923.0</v>
+        <v>43923</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>80</v>
@@ -1700,7 +1719,7 @@
         <v>32</v>
       </c>
       <c r="J8" s="4">
-        <v>87.0</v>
+        <v>87</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>42</v>
@@ -1709,10 +1728,13 @@
         <v>43</v>
       </c>
       <c r="M8" s="4">
-        <v>360.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>360</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>81</v>
       </c>
@@ -1729,10 +1751,10 @@
         <v>84</v>
       </c>
       <c r="F9" s="3">
-        <v>43996.0</v>
+        <v>43996</v>
       </c>
       <c r="G9" s="3">
-        <v>43914.0</v>
+        <v>43914</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>50</v>
@@ -1741,7 +1763,7 @@
         <v>85</v>
       </c>
       <c r="J9" s="4">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>23</v>
@@ -1750,10 +1772,13 @@
         <v>74</v>
       </c>
       <c r="M9" s="4">
-        <v>162.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>162</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>87</v>
       </c>
@@ -1770,10 +1795,10 @@
         <v>49</v>
       </c>
       <c r="F10" s="3">
-        <v>43996.0</v>
+        <v>43996</v>
       </c>
       <c r="G10" s="3">
-        <v>44284.0</v>
+        <v>44284</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>70</v>
@@ -1782,7 +1807,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="4">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>42</v>
@@ -1791,27 +1816,31 @@
         <v>93</v>
       </c>
       <c r="M10" s="4">
-        <v>181.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>181</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>98</v>
       </c>
+      <c r="D11" s="10"/>
       <c r="E11" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F11" s="3">
-        <v>43704.0</v>
+        <v>43704</v>
       </c>
       <c r="G11" s="3">
-        <v>44015.0</v>
+        <v>44015</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>101</v>
@@ -1820,7 +1849,7 @@
         <v>85</v>
       </c>
       <c r="J11" s="4">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>42</v>
@@ -1829,10 +1858,13 @@
         <v>74</v>
       </c>
       <c r="M11" s="4">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>200</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>104</v>
       </c>
@@ -1849,10 +1881,10 @@
         <v>84</v>
       </c>
       <c r="F12" s="3">
-        <v>43703.0</v>
+        <v>43703</v>
       </c>
       <c r="G12" s="3">
-        <v>44117.0</v>
+        <v>44117</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>109</v>
@@ -1861,7 +1893,7 @@
         <v>110</v>
       </c>
       <c r="J12" s="4">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>42</v>
@@ -1870,10 +1902,13 @@
         <v>52</v>
       </c>
       <c r="M12" s="4">
-        <v>339.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>339</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>113</v>
       </c>
@@ -1890,10 +1925,10 @@
         <v>74</v>
       </c>
       <c r="F13" s="3">
-        <v>43947.0</v>
+        <v>43947</v>
       </c>
       <c r="G13" s="3">
-        <v>43749.0</v>
+        <v>43749</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>80</v>
@@ -1902,7 +1937,7 @@
         <v>92</v>
       </c>
       <c r="J13" s="4">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>23</v>
@@ -1911,10 +1946,13 @@
         <v>93</v>
       </c>
       <c r="M13" s="4">
-        <v>301.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>301</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>120</v>
       </c>
@@ -1931,10 +1969,10 @@
         <v>24</v>
       </c>
       <c r="F14" s="3">
-        <v>43753.0</v>
+        <v>43753</v>
       </c>
       <c r="G14" s="3">
-        <v>44042.0</v>
+        <v>44042</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>31</v>
@@ -1943,7 +1981,7 @@
         <v>51</v>
       </c>
       <c r="J14" s="4">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>42</v>
@@ -1952,10 +1990,13 @@
         <v>62</v>
       </c>
       <c r="M14" s="4">
-        <v>295.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>295</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>125</v>
       </c>
@@ -1972,10 +2013,10 @@
         <v>58</v>
       </c>
       <c r="F15" s="3">
-        <v>44002.0</v>
+        <v>44002</v>
       </c>
       <c r="G15" s="3">
-        <v>43741.0</v>
+        <v>43741</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>70</v>
@@ -1984,7 +2025,7 @@
         <v>22</v>
       </c>
       <c r="J15" s="4">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>23</v>
@@ -1993,10 +2034,13 @@
         <v>84</v>
       </c>
       <c r="M15" s="4">
-        <v>155.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>155</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>132</v>
       </c>
@@ -2013,10 +2057,10 @@
         <v>62</v>
       </c>
       <c r="F16" s="3">
-        <v>44266.0</v>
+        <v>44266</v>
       </c>
       <c r="G16" s="3">
-        <v>44065.0</v>
+        <v>44065</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>135</v>
@@ -2025,7 +2069,7 @@
         <v>41</v>
       </c>
       <c r="J16" s="4">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>42</v>
@@ -2034,10 +2078,13 @@
         <v>62</v>
       </c>
       <c r="M16" s="4">
-        <v>288.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>288</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>136</v>
       </c>
@@ -2054,10 +2101,10 @@
         <v>58</v>
       </c>
       <c r="F17" s="3">
-        <v>44313.0</v>
+        <v>44313</v>
       </c>
       <c r="G17" s="3">
-        <v>44115.0</v>
+        <v>44115</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>101</v>
@@ -2066,7 +2113,7 @@
         <v>22</v>
       </c>
       <c r="J17" s="4">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>42</v>
@@ -2075,10 +2122,13 @@
         <v>49</v>
       </c>
       <c r="M17" s="4">
-        <v>339.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>339</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>139</v>
       </c>
@@ -2095,10 +2145,10 @@
         <v>62</v>
       </c>
       <c r="F18" s="3">
-        <v>43863.0</v>
+        <v>43863</v>
       </c>
       <c r="G18" s="3">
-        <v>43921.0</v>
+        <v>43921</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>80</v>
@@ -2107,7 +2157,7 @@
         <v>110</v>
       </c>
       <c r="J18" s="4">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>23</v>
@@ -2116,10 +2166,13 @@
         <v>62</v>
       </c>
       <c r="M18" s="4">
-        <v>157.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>157</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>142</v>
       </c>
@@ -2136,10 +2189,10 @@
         <v>84</v>
       </c>
       <c r="F19" s="3">
-        <v>44287.0</v>
+        <v>44287</v>
       </c>
       <c r="G19" s="3">
-        <v>44135.0</v>
+        <v>44135</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>135</v>
@@ -2148,7 +2201,7 @@
         <v>22</v>
       </c>
       <c r="J19" s="4">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>23</v>
@@ -2157,27 +2210,31 @@
         <v>19</v>
       </c>
       <c r="M19" s="4">
-        <v>371.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>371</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="9" t="s">
         <v>148</v>
       </c>
+      <c r="D20" s="10"/>
       <c r="E20" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F20" s="3">
-        <v>43904.0</v>
+        <v>43904</v>
       </c>
       <c r="G20" s="3">
-        <v>44220.0</v>
+        <v>44220</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>70</v>
@@ -2186,7 +2243,7 @@
         <v>92</v>
       </c>
       <c r="J20" s="4">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>23</v>
@@ -2195,7 +2252,10 @@
         <v>49</v>
       </c>
       <c r="M20" s="4">
-        <v>177.0</v>
+        <v>177</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -2204,73 +2264,80 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C20:D20"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.86"/>
-    <col customWidth="1" min="2" max="2" width="25.86"/>
-    <col customWidth="1" min="3" max="3" width="34.14"/>
-    <col customWidth="1" min="5" max="5" width="22.29"/>
+    <col min="1" max="1" width="30.83203125" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34.1640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2287,7 +2354,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2298,13 +2365,13 @@
         <v>48</v>
       </c>
       <c r="D2" s="4">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="E2" s="4">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -2315,13 +2382,13 @@
         <v>54</v>
       </c>
       <c r="D3" s="4">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2332,13 +2399,13 @@
         <v>60</v>
       </c>
       <c r="D4" s="4">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="E4" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -2349,13 +2416,13 @@
         <v>65</v>
       </c>
       <c r="D5" s="4">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="E5" s="4">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2366,13 +2433,13 @@
         <v>69</v>
       </c>
       <c r="D6" s="4">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="E6" s="4">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
@@ -2383,13 +2450,13 @@
         <v>72</v>
       </c>
       <c r="D7" s="4">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>74</v>
       </c>
@@ -2400,13 +2467,13 @@
         <v>76</v>
       </c>
       <c r="D8" s="4">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="E8" s="4">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -2417,13 +2484,13 @@
         <v>86</v>
       </c>
       <c r="D9" s="4">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="E9" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2434,13 +2501,13 @@
         <v>91</v>
       </c>
       <c r="D10" s="4">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="E10" s="4">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>93</v>
       </c>
@@ -2451,13 +2518,13 @@
         <v>95</v>
       </c>
       <c r="D11" s="4">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
@@ -2468,13 +2535,13 @@
         <v>100</v>
       </c>
       <c r="D12" s="4">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="E12" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -2485,13 +2552,13 @@
         <v>103</v>
       </c>
       <c r="D13" s="4">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E13" s="4">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>34</v>
       </c>
@@ -2502,13 +2569,13 @@
         <v>108</v>
       </c>
       <c r="D14" s="4">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>93</v>
       </c>
@@ -2519,13 +2586,13 @@
         <v>112</v>
       </c>
       <c r="D15" s="4">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="E15" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
@@ -2536,13 +2603,13 @@
         <v>117</v>
       </c>
       <c r="D16" s="4">
-        <v>89.0</v>
+        <v>89</v>
       </c>
       <c r="E16" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -2553,13 +2620,13 @@
         <v>119</v>
       </c>
       <c r="D17" s="4">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="E17" s="4">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -2570,13 +2637,13 @@
         <v>124</v>
       </c>
       <c r="D18" s="4">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -2587,13 +2654,13 @@
         <v>129</v>
       </c>
       <c r="D19" s="4">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="E19" s="4">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>58</v>
       </c>
@@ -2604,32 +2671,35 @@
         <v>131</v>
       </c>
       <c r="D20" s="4">
-        <v>90.0</v>
+        <v>90</v>
       </c>
       <c r="E20" s="4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="15.86"/>
-    <col customWidth="1" min="6" max="6" width="30.86"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -2656,7 +2726,7 @@
       </c>
       <c r="I1" s="6"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>153</v>
       </c>
@@ -2676,13 +2746,14 @@
         <v>19</v>
       </c>
       <c r="G2" s="3">
-        <v>38261.0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>43572.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>38261</v>
+      </c>
+      <c r="H2" s="11">
+        <v>43572</v>
+      </c>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>156</v>
       </c>
@@ -2702,13 +2773,14 @@
         <v>84</v>
       </c>
       <c r="G3" s="7">
-        <v>44334.0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>39039.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>44334</v>
+      </c>
+      <c r="H3" s="11">
+        <v>39039</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>160</v>
       </c>
@@ -2728,13 +2800,14 @@
         <v>49</v>
       </c>
       <c r="G4" s="3">
-        <v>39685.0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>39760.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>39685</v>
+      </c>
+      <c r="H4" s="11">
+        <v>39760</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>164</v>
       </c>
@@ -2754,14 +2827,14 @@
         <v>49</v>
       </c>
       <c r="G5" s="3">
-        <v>40180.0</v>
+        <v>40180</v>
       </c>
       <c r="H5" s="3">
-        <v>40003.0</v>
+        <v>40003</v>
       </c>
       <c r="I5" s="6"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>167</v>
       </c>
@@ -2781,13 +2854,14 @@
         <v>84</v>
       </c>
       <c r="G6" s="3">
-        <v>39280.0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>36827.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>39280</v>
+      </c>
+      <c r="H6" s="11">
+        <v>36827</v>
+      </c>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>170</v>
       </c>
@@ -2807,13 +2881,14 @@
         <v>84</v>
       </c>
       <c r="G7" s="3">
-        <v>41429.0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>37144.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>41429</v>
+      </c>
+      <c r="H7" s="11">
+        <v>37144</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>173</v>
       </c>
@@ -2833,13 +2908,14 @@
         <v>34</v>
       </c>
       <c r="G8" s="3">
-        <v>37126.0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>40588.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>37126</v>
+      </c>
+      <c r="H8" s="11">
+        <v>40588</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>176</v>
       </c>
@@ -2859,13 +2935,14 @@
         <v>34</v>
       </c>
       <c r="G9" s="3">
-        <v>42218.0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>39793.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>42218</v>
+      </c>
+      <c r="H9" s="11">
+        <v>39793</v>
+      </c>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>179</v>
       </c>
@@ -2885,13 +2962,14 @@
         <v>74</v>
       </c>
       <c r="G10" s="3">
-        <v>40435.0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>42487.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>40435</v>
+      </c>
+      <c r="H10" s="11">
+        <v>42487</v>
+      </c>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>182</v>
       </c>
@@ -2911,13 +2989,14 @@
         <v>34</v>
       </c>
       <c r="G11" s="3">
-        <v>38949.0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>42612.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>38949</v>
+      </c>
+      <c r="H11" s="11">
+        <v>42612</v>
+      </c>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>185</v>
       </c>
@@ -2937,13 +3016,14 @@
         <v>58</v>
       </c>
       <c r="G12" s="7">
-        <v>37027.0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>40903.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>37027</v>
+      </c>
+      <c r="H12" s="11">
+        <v>40903</v>
+      </c>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>189</v>
       </c>
@@ -2963,13 +3043,14 @@
         <v>62</v>
       </c>
       <c r="G13" s="3">
-        <v>43762.0</v>
-      </c>
-      <c r="H13" s="7">
-        <v>43247.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>43762</v>
+      </c>
+      <c r="H13" s="12">
+        <v>43247</v>
+      </c>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>192</v>
       </c>
@@ -2989,13 +3070,14 @@
         <v>62</v>
       </c>
       <c r="G14" s="7">
-        <v>38838.0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>41465.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>38838</v>
+      </c>
+      <c r="H14" s="11">
+        <v>41465</v>
+      </c>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>195</v>
       </c>
@@ -3015,13 +3097,14 @@
         <v>49</v>
       </c>
       <c r="G15" s="7">
-        <v>37029.0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>39318.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>37029</v>
+      </c>
+      <c r="H15" s="11">
+        <v>39318</v>
+      </c>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>197</v>
       </c>
@@ -3041,13 +3124,14 @@
         <v>43</v>
       </c>
       <c r="G16" s="3">
-        <v>38808.0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>41430.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>38808</v>
+      </c>
+      <c r="H16" s="11">
+        <v>41430</v>
+      </c>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>200</v>
       </c>
@@ -3067,13 +3151,14 @@
         <v>93</v>
       </c>
       <c r="G17" s="3">
-        <v>38414.0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>42968.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>38414</v>
+      </c>
+      <c r="H17" s="11">
+        <v>42968</v>
+      </c>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>203</v>
       </c>
@@ -3093,13 +3178,14 @@
         <v>49</v>
       </c>
       <c r="G18" s="3">
-        <v>38300.0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>44257.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>38300</v>
+      </c>
+      <c r="H18" s="11">
+        <v>44257</v>
+      </c>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>206</v>
       </c>
@@ -3119,13 +3205,14 @@
         <v>58</v>
       </c>
       <c r="G19" s="3">
-        <v>42443.0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>39497.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>42443</v>
+      </c>
+      <c r="H19" s="11">
+        <v>39497</v>
+      </c>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>209</v>
       </c>
@@ -3145,24 +3232,15 @@
         <v>52</v>
       </c>
       <c r="G20" s="3">
-        <v>37420.0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>36838.0</v>
-      </c>
+        <v>37420</v>
+      </c>
+      <c r="H20" s="11">
+        <v>36838</v>
+      </c>
+      <c r="I20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="H11:I11"/>
@@ -3171,27 +3249,38 @@
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H16:I16"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.71"/>
-    <col customWidth="1" min="2" max="2" width="8.14"/>
-    <col customWidth="1" min="6" max="6" width="30.86"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>214</v>
       </c>
@@ -3218,7 +3307,7 @@
       </c>
       <c r="I1" s="6"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>219</v>
       </c>
@@ -3238,13 +3327,14 @@
         <v>84</v>
       </c>
       <c r="G2" s="3">
-        <v>43626.0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>42962.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>43626</v>
+      </c>
+      <c r="H2" s="11">
+        <v>42962</v>
+      </c>
+      <c r="I2" s="10"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>223</v>
       </c>
@@ -3264,13 +3354,14 @@
         <v>24</v>
       </c>
       <c r="G3" s="3">
-        <v>40725.0</v>
-      </c>
-      <c r="H3" s="3">
-        <v>40348.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>40725</v>
+      </c>
+      <c r="H3" s="11">
+        <v>40348</v>
+      </c>
+      <c r="I3" s="10"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>262</v>
       </c>
@@ -3290,13 +3381,14 @@
         <v>24</v>
       </c>
       <c r="G4" s="3">
-        <v>43585.0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>42014.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>43585</v>
+      </c>
+      <c r="H4" s="11">
+        <v>42014</v>
+      </c>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>285</v>
       </c>
@@ -3316,13 +3408,14 @@
         <v>24</v>
       </c>
       <c r="G5" s="3">
-        <v>38775.0</v>
-      </c>
-      <c r="H5" s="3">
-        <v>44130.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>38775</v>
+      </c>
+      <c r="H5" s="11">
+        <v>44130</v>
+      </c>
+      <c r="I5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>295</v>
       </c>
@@ -3342,13 +3435,14 @@
         <v>58</v>
       </c>
       <c r="G6" s="3">
-        <v>37410.0</v>
-      </c>
-      <c r="H6" s="3">
-        <v>40076.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>37410</v>
+      </c>
+      <c r="H6" s="11">
+        <v>40076</v>
+      </c>
+      <c r="I6" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>312</v>
       </c>
@@ -3368,13 +3462,14 @@
         <v>74</v>
       </c>
       <c r="G7" s="3">
-        <v>36705.0</v>
-      </c>
-      <c r="H7" s="3">
-        <v>38784.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>36705</v>
+      </c>
+      <c r="H7" s="11">
+        <v>38784</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>315</v>
       </c>
@@ -3394,13 +3489,14 @@
         <v>49</v>
       </c>
       <c r="G8" s="3">
-        <v>37775.0</v>
-      </c>
-      <c r="H8" s="3">
-        <v>40568.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>37775</v>
+      </c>
+      <c r="H8" s="11">
+        <v>40568</v>
+      </c>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>318</v>
       </c>
@@ -3420,13 +3516,14 @@
         <v>84</v>
       </c>
       <c r="G9" s="7">
-        <v>44338.0</v>
-      </c>
-      <c r="H9" s="3">
-        <v>38142.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>44338</v>
+      </c>
+      <c r="H9" s="11">
+        <v>38142</v>
+      </c>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>321</v>
       </c>
@@ -3446,13 +3543,14 @@
         <v>58</v>
       </c>
       <c r="G10" s="3">
-        <v>43638.0</v>
-      </c>
-      <c r="H10" s="3">
-        <v>43530.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>43638</v>
+      </c>
+      <c r="H10" s="11">
+        <v>43530</v>
+      </c>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>323</v>
       </c>
@@ -3472,13 +3570,14 @@
         <v>62</v>
       </c>
       <c r="G11" s="3">
-        <v>41435.0</v>
-      </c>
-      <c r="H11" s="3">
-        <v>37572.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>41435</v>
+      </c>
+      <c r="H11" s="11">
+        <v>37572</v>
+      </c>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>326</v>
       </c>
@@ -3498,13 +3597,14 @@
         <v>93</v>
       </c>
       <c r="G12" s="3">
-        <v>41092.0</v>
-      </c>
-      <c r="H12" s="3">
-        <v>37353.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>41092</v>
+      </c>
+      <c r="H12" s="11">
+        <v>37353</v>
+      </c>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>329</v>
       </c>
@@ -3524,13 +3624,14 @@
         <v>84</v>
       </c>
       <c r="G13" s="7">
-        <v>42858.0</v>
-      </c>
-      <c r="H13" s="3">
-        <v>43120.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>42858</v>
+      </c>
+      <c r="H13" s="11">
+        <v>43120</v>
+      </c>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>332</v>
       </c>
@@ -3550,13 +3651,14 @@
         <v>74</v>
       </c>
       <c r="G14" s="3">
-        <v>40493.0</v>
-      </c>
-      <c r="H14" s="3">
-        <v>38804.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>40493</v>
+      </c>
+      <c r="H14" s="11">
+        <v>38804</v>
+      </c>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>335</v>
       </c>
@@ -3576,13 +3678,14 @@
         <v>58</v>
       </c>
       <c r="G15" s="3">
-        <v>43007.0</v>
-      </c>
-      <c r="H15" s="3">
-        <v>42464.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>43007</v>
+      </c>
+      <c r="H15" s="11">
+        <v>42464</v>
+      </c>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>338</v>
       </c>
@@ -3602,13 +3705,14 @@
         <v>93</v>
       </c>
       <c r="G16" s="3">
-        <v>38021.0</v>
-      </c>
-      <c r="H16" s="3">
-        <v>41112.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>38021</v>
+      </c>
+      <c r="H16" s="11">
+        <v>41112</v>
+      </c>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>341</v>
       </c>
@@ -3628,13 +3732,14 @@
         <v>43</v>
       </c>
       <c r="G17" s="3">
-        <v>40427.0</v>
-      </c>
-      <c r="H17" s="3">
-        <v>43949.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>40427</v>
+      </c>
+      <c r="H17" s="11">
+        <v>43949</v>
+      </c>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>344</v>
       </c>
@@ -3654,13 +3759,14 @@
         <v>74</v>
       </c>
       <c r="G18" s="3">
-        <v>41944.0</v>
-      </c>
-      <c r="H18" s="3">
-        <v>41818.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>41944</v>
+      </c>
+      <c r="H18" s="11">
+        <v>41818</v>
+      </c>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>347</v>
       </c>
@@ -3680,13 +3786,14 @@
         <v>58</v>
       </c>
       <c r="G19" s="3">
-        <v>41935.0</v>
-      </c>
-      <c r="H19" s="3">
-        <v>38409.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>41935</v>
+      </c>
+      <c r="H19" s="11">
+        <v>38409</v>
+      </c>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>350</v>
       </c>
@@ -3706,24 +3813,15 @@
         <v>34</v>
       </c>
       <c r="G20" s="3">
-        <v>43298.0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>39466.0</v>
-      </c>
+        <v>43298</v>
+      </c>
+      <c r="H20" s="11">
+        <v>39466</v>
+      </c>
+      <c r="I20" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="H20:I20"/>
@@ -3733,25 +3831,36 @@
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.71"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>212</v>
       </c>
@@ -3768,7 +3877,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>216</v>
       </c>
@@ -3785,7 +3894,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>230</v>
       </c>
@@ -3802,7 +3911,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>234</v>
       </c>
@@ -3819,7 +3928,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>237</v>
       </c>
@@ -3836,7 +3945,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>242</v>
       </c>
@@ -3853,7 +3962,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>246</v>
       </c>
@@ -3870,7 +3979,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>250</v>
       </c>
@@ -3887,7 +3996,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>254</v>
       </c>
@@ -3904,7 +4013,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>258</v>
       </c>
@@ -3921,7 +4030,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>263</v>
       </c>
@@ -3938,7 +4047,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>268</v>
       </c>
@@ -3955,7 +4064,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>273</v>
       </c>
@@ -3972,7 +4081,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>277</v>
       </c>
@@ -3989,7 +4098,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>281</v>
       </c>
@@ -4006,7 +4115,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>288</v>
       </c>
@@ -4023,7 +4132,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>292</v>
       </c>
@@ -4040,7 +4149,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>298</v>
       </c>
@@ -4057,7 +4166,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>303</v>
       </c>
@@ -4074,7 +4183,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>308</v>
       </c>
@@ -4092,6 +4201,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Document for phase 2
</commit_message>
<xml_diff>
--- a/Documentation/Sample Data for Hospital Database.xlsx
+++ b/Documentation/Sample Data for Hospital Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Spencer/Documents/CMSC508/Project/vcu-cs-cmsc508-teamproject-summer2020-team-10/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D96F24B-8E96-D343-B38C-3BD810770005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB8C9FD-0040-6B48-806E-5E418A49D14A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="291">
   <si>
     <t>Emergency</t>
   </si>
@@ -906,7 +906,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yy"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -918,16 +918,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1003,9 +1006,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
@@ -1228,7 +1231,7 @@
   </sheetPr>
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -1241,7 +1244,7 @@
     <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>242</v>
       </c>
@@ -2213,8 +2216,8 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2261,9 +2264,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="A9" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="15" t="s">
@@ -2282,7 +2283,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2822,7 +2823,7 @@
   </sheetPr>
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -3685,7 +3686,7 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>

</xml_diff>